<commit_message>
Auto update excel for corona report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2020-12-20.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2020-12-20.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -117,10 +117,10 @@
     <t xml:space="preserve">187</t>
   </si>
   <si>
-    <t xml:space="preserve">206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,2 %</t>
+    <t xml:space="preserve">207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Unter-60-Jährige</t>
@@ -129,7 +129,7 @@
     <t xml:space="preserve">191</t>
   </si>
   <si>
-    <t xml:space="preserve"> 7,9 %</t>
+    <t xml:space="preserve"> 8,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">Über-60-Jährige</t>
@@ -138,10 +138,10 @@
     <t xml:space="preserve">177</t>
   </si>
   <si>
-    <t xml:space="preserve">203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,7 %</t>
+    <t xml:space="preserve">204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 60-bis-79-Jährige</t>
@@ -150,10 +150,10 @@
     <t xml:space="preserve">132</t>
   </si>
   <si>
-    <t xml:space="preserve">154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,7 %</t>
+    <t xml:space="preserve">155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,4 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon Über-80-Jährige</t>
@@ -162,7 +162,10 @@
     <t xml:space="preserve">323</t>
   </si>
   <si>
-    <t xml:space="preserve">362</t>
+    <t xml:space="preserve">364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Regionen mit 7-TI bei Über-60-Jährigen:</t>
@@ -174,10 +177,7 @@
     <t xml:space="preserve">385</t>
   </si>
   <si>
-    <t xml:space="preserve">391</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1,6 %</t>
+    <t xml:space="preserve">392</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; 50</t>
@@ -186,10 +186,10 @@
     <t xml:space="preserve">374</t>
   </si>
   <si>
-    <t xml:space="preserve">381</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1,9 %</t>
+    <t xml:space="preserve">382</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,1 %</t>
   </si>
   <si>
     <t xml:space="preserve">Intensivbetten</t>
@@ -241,19 +241,25 @@
     <t xml:space="preserve">Ohne Symptomatik</t>
   </si>
   <si>
-    <t xml:space="preserve">15,6 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> %</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PP</t>
+    <t xml:space="preserve">15 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,5 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Nicht stationär behandelt</t>
   </si>
   <si>
-    <t xml:space="preserve">92,7 %</t>
+    <t xml:space="preserve">91,3 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">92,2 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,9 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Intensivmedizinisch behandelt (Schätzung)</t>
@@ -352,46 +358,46 @@
     <t xml:space="preserve">78 ( 0,1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">76 ( 0,1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -2,6%</t>
+    <t xml:space="preserve">75 ( 0,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -3,8%</t>
   </si>
   <si>
     <t xml:space="preserve">60 bis 79 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">538 ( 3,1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">643 ( 3,5%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  19,5%</t>
+    <t xml:space="preserve">542 ( 3,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">656 ( 3,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  21,0%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
   </si>
   <si>
-    <t xml:space="preserve">1466 (16,4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1794 (16,7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  22,4%</t>
+    <t xml:space="preserve">1485 (16,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1820 (16,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  22,6%</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">2084 ( 1,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2513 ( 2,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  20,6%</t>
+    <t xml:space="preserve">2107 ( 1,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2552 ( 2,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  21,1%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
@@ -421,9 +427,6 @@
     <t xml:space="preserve">1665 (16,3%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  -3,8%</t>
-  </si>
-  <si>
     <t xml:space="preserve">1540 ( 8,6%)</t>
   </si>
   <si>
@@ -442,7 +445,7 @@
     <t xml:space="preserve">16 Tage</t>
   </si>
   <si>
-    <t xml:space="preserve">13 Tage</t>
+    <t xml:space="preserve">12 Tage</t>
   </si>
   <si>
     <t xml:space="preserve">kürzeste</t>
@@ -1192,12 +1195,12 @@
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1205,16 +1208,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -1351,29 +1354,29 @@
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1381,47 +1384,47 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1429,58 +1432,58 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" t="s">
         <v>101</v>
-      </c>
-      <c r="D12" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1499,13 +1502,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1513,63 +1516,63 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
@@ -1577,58 +1580,58 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1650,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1661,27 +1664,27 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D2" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D3" t="n">
         <v>-1</v>
@@ -1689,13 +1692,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" t="n">
         <v>-6</v>
@@ -1717,50 +1720,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2" t="n">
         <v>1.11</v>
       </c>
       <c r="C2" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D2" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B3" t="n">
         <v>1.09</v>
       </c>
       <c r="C3" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D3" t="n">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E3" t="n">
         <v>9</v>
@@ -1768,16 +1771,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B4" t="n">
         <v>1.07</v>
       </c>
       <c r="C4" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D4" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E4" t="n">
         <v>9</v>
@@ -1785,16 +1788,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B5" t="n">
         <v>1.03</v>
       </c>
       <c r="C5" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D5" t="n">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E5" t="n">
         <v>16</v>
@@ -1802,16 +1805,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B6" t="n">
         <v>1.19</v>
       </c>
       <c r="C6" t="n">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D6" t="n">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E6" t="n">
         <v>10</v>
@@ -1819,7 +1822,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B7" t="n">
         <v>1.06</v>
@@ -1828,41 +1831,41 @@
         <v>130</v>
       </c>
       <c r="D7" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E7" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B8" t="n">
         <v>1.16</v>
       </c>
       <c r="C8" t="n">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D8" t="n">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9" t="n">
         <v>1.1</v>
       </c>
       <c r="C9" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D9" t="n">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
@@ -1870,13 +1873,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B10" t="n">
         <v>1.25</v>
       </c>
       <c r="C10" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D10" t="n">
         <v>89</v>
@@ -1887,7 +1890,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B11" t="n">
         <v>1.14</v>
@@ -1904,7 +1907,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B12" t="n">
         <v>1.11</v>
@@ -1921,16 +1924,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B13" t="n">
         <v>1.11</v>
       </c>
       <c r="C13" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D13" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E13" t="n">
         <v>16</v>
@@ -1938,16 +1941,16 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B14" t="n">
         <v>1.12</v>
       </c>
       <c r="C14" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D14" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E14" t="n">
         <v>29</v>
@@ -1955,16 +1958,16 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B15" t="n">
         <v>1.18</v>
       </c>
       <c r="C15" t="n">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="D15" t="n">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="E15" t="n">
         <v>4</v>
@@ -1972,16 +1975,16 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B16" t="n">
         <v>1.1</v>
       </c>
       <c r="C16" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D16" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E16" t="n">
         <v>17</v>
@@ -1989,33 +1992,33 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B17" t="n">
         <v>1.27</v>
       </c>
       <c r="C17" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D17" t="n">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E17" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B18" t="n">
         <v>1.22</v>
       </c>
       <c r="C18" t="n">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D18" t="n">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E18" t="n">
         <v>8</v>
@@ -2037,112 +2040,112 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C2" t="n">
         <v>624140</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F2" t="n">
         <v>68799</v>
       </c>
       <c r="G2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H2" t="n">
         <v>782</v>
       </c>
       <c r="I2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C3" t="n">
         <v>625930</v>
       </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F3" t="n">
         <v>67503</v>
       </c>
       <c r="G3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H3" t="n">
         <v>723</v>
       </c>
       <c r="I3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C4" t="n">
         <v>700322</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -2151,181 +2154,181 @@
         <v>18626</v>
       </c>
       <c r="G4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H4" t="n">
         <v>472</v>
       </c>
       <c r="I4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C5" t="n">
         <v>2529756</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F5" t="n">
         <v>48926</v>
       </c>
       <c r="G5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H5" t="n">
         <v>401</v>
       </c>
       <c r="I5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C6" t="n">
         <v>1797236</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F6" t="n">
         <v>14394</v>
       </c>
       <c r="G6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H6" t="n">
         <v>384</v>
       </c>
       <c r="I6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C7" t="n">
         <v>1953185</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F7" t="n">
         <v>60665</v>
       </c>
       <c r="G7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H7" t="n">
         <v>370</v>
       </c>
       <c r="I7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C8" t="n">
         <v>1202700</v>
       </c>
       <c r="D8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F8" t="n">
         <v>25397</v>
       </c>
       <c r="G8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H8" t="n">
         <v>368</v>
       </c>
       <c r="I8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C9" t="n">
         <v>591294</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F9" t="n">
         <v>26400</v>
       </c>
       <c r="G9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H9" t="n">
         <v>296</v>
       </c>
       <c r="I9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -2334,57 +2337,57 @@
         <v>2046161</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F10" t="n">
         <v>10331</v>
       </c>
       <c r="G10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H10" t="n">
         <v>280</v>
       </c>
       <c r="I10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" t="n">
         <v>1514962</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F11" t="n">
         <v>10578</v>
       </c>
       <c r="G11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H11" t="n">
         <v>241</v>
       </c>
       <c r="I11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>